<commit_message>
Dummy data attractions done
</commit_message>
<xml_diff>
--- a/data/Dummy Data.xlsx
+++ b/data/Dummy Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\0001 MY COURSES\0000 Computer Science\COMP 346 - Internet Computing\346-term-project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\0001 MY COURSES\0000 Computer Science\COMP 346 - Internet Computing\346-term-project\Github\danglingpointers\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="153">
   <si>
     <t>Chicago</t>
   </si>
@@ -345,9 +345,6 @@
     <t>The Houston Zoo</t>
   </si>
   <si>
-    <t>Screamworld Haunted Houses of Houston</t>
-  </si>
-  <si>
     <t>Discovery Green</t>
   </si>
   <si>
@@ -378,9 +375,6 @@
     <t>Landmarks</t>
   </si>
   <si>
-    <t>Williams Waterfall</t>
-  </si>
-  <si>
     <t>Eleanor Tinsley Park</t>
   </si>
   <si>
@@ -403,6 +397,93 @@
   </si>
   <si>
     <t>Musee Mecanique</t>
+  </si>
+  <si>
+    <t>California Academy of Sciences</t>
+  </si>
+  <si>
+    <t>Alcatraz Island</t>
+  </si>
+  <si>
+    <t>The Walt Disney Family Museum</t>
+  </si>
+  <si>
+    <t>Conservatory of Flowers</t>
+  </si>
+  <si>
+    <t>Exploratorium</t>
+  </si>
+  <si>
+    <t>Palace of Fine Arts</t>
+  </si>
+  <si>
+    <t>Lombard Street</t>
+  </si>
+  <si>
+    <t>San Francisco Zoo</t>
+  </si>
+  <si>
+    <t>Randall Museum</t>
+  </si>
+  <si>
+    <t>Golden Gate Bridge</t>
+  </si>
+  <si>
+    <t>Castro Theatre</t>
+  </si>
+  <si>
+    <t>San Francisco Giants</t>
+  </si>
+  <si>
+    <t>Millenium Park</t>
+  </si>
+  <si>
+    <t>Navy Pier</t>
+  </si>
+  <si>
+    <t>Willis Tower</t>
+  </si>
+  <si>
+    <t>Buckingham Fountain</t>
+  </si>
+  <si>
+    <t>Lincoln Park Zoo</t>
+  </si>
+  <si>
+    <t>Museum of Science and Industry</t>
+  </si>
+  <si>
+    <t>The Field Museum</t>
+  </si>
+  <si>
+    <t>Chicago Cultural Center</t>
+  </si>
+  <si>
+    <t>360 Chicago</t>
+  </si>
+  <si>
+    <t>The Art Institute of Chicago</t>
+  </si>
+  <si>
+    <t>The Cloud Gate aka the 'Bean'</t>
+  </si>
+  <si>
+    <t>Chicago Architechture Foundation</t>
+  </si>
+  <si>
+    <t>Haunted Sanitarium</t>
+  </si>
+  <si>
+    <t>Chicago Bulls</t>
+  </si>
+  <si>
+    <t>Fear City Haunted House</t>
+  </si>
+  <si>
+    <t>Menil Park</t>
+  </si>
+  <si>
+    <t>Gerald D. Hines Waterfall</t>
   </si>
 </sst>
 </file>
@@ -1539,7 +1620,7 @@
   <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1575,7 +1656,15 @@
       <c r="B2" t="s">
         <v>102</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="C2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2" s="3">
+        <v>41.882551999999997</v>
+      </c>
+      <c r="E2">
+        <v>-87.622551000000001</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1584,7 +1673,15 @@
       <c r="B3" t="s">
         <v>104</v>
       </c>
-      <c r="D3" s="3"/>
+      <c r="C3" t="s">
+        <v>140</v>
+      </c>
+      <c r="D3" s="3">
+        <v>41.92089</v>
+      </c>
+      <c r="E3">
+        <v>-87.632917000000006</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1593,117 +1690,221 @@
       <c r="B4" t="s">
         <v>102</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="C4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D4" s="3">
+        <v>41.891641999999997</v>
+      </c>
+      <c r="E4">
+        <v>-87.605143999999996</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>102</v>
-      </c>
-      <c r="D5" s="3"/>
+        <v>115</v>
+      </c>
+      <c r="C5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D5" s="3">
+        <v>41.882657000000002</v>
+      </c>
+      <c r="E5">
+        <v>-87.623304000000005</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>108</v>
-      </c>
-      <c r="D6" s="3"/>
+        <v>107</v>
+      </c>
+      <c r="C6" t="s">
+        <v>150</v>
+      </c>
+      <c r="D6" s="3">
+        <v>42.031595000000003</v>
+      </c>
+      <c r="E6">
+        <v>-87.779088000000002</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>110</v>
-      </c>
-      <c r="D7" s="3"/>
+        <v>109</v>
+      </c>
+      <c r="C7" t="s">
+        <v>141</v>
+      </c>
+      <c r="D7" s="3">
+        <v>41.790573000000002</v>
+      </c>
+      <c r="E7">
+        <v>-87.583066000000002</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>110</v>
-      </c>
-      <c r="D8" s="3"/>
+        <v>109</v>
+      </c>
+      <c r="C8" t="s">
+        <v>142</v>
+      </c>
+      <c r="D8" s="3">
+        <v>41.866261000000002</v>
+      </c>
+      <c r="E8">
+        <v>-87.616979999999998</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>110</v>
-      </c>
-      <c r="D9" s="3"/>
+        <v>109</v>
+      </c>
+      <c r="C9" t="s">
+        <v>143</v>
+      </c>
+      <c r="D9" s="3">
+        <v>41.883754000000003</v>
+      </c>
+      <c r="E9">
+        <v>-87.624951999999993</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>102</v>
-      </c>
-      <c r="D10" s="3"/>
+        <v>115</v>
+      </c>
+      <c r="C10" t="s">
+        <v>139</v>
+      </c>
+      <c r="D10" s="3">
+        <v>41.875793999999999</v>
+      </c>
+      <c r="E10">
+        <v>-87.618948000000003</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>110</v>
-      </c>
-      <c r="D11" s="3"/>
+        <v>109</v>
+      </c>
+      <c r="C11" t="s">
+        <v>145</v>
+      </c>
+      <c r="D11" s="3">
+        <v>41.879584000000001</v>
+      </c>
+      <c r="E11">
+        <v>-87.623712999999995</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>116</v>
-      </c>
-      <c r="D12" s="3"/>
+        <v>115</v>
+      </c>
+      <c r="C12" t="s">
+        <v>138</v>
+      </c>
+      <c r="D12" s="3">
+        <v>41.878875999999998</v>
+      </c>
+      <c r="E12">
+        <v>-87.635914999999997</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>102</v>
-      </c>
-      <c r="D13" s="3"/>
+        <v>115</v>
+      </c>
+      <c r="C13" t="s">
+        <v>144</v>
+      </c>
+      <c r="D13" s="3">
+        <v>41.898510000000002</v>
+      </c>
+      <c r="E13">
+        <v>-87.622765000000001</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>110</v>
-      </c>
-      <c r="D14" s="3"/>
+        <v>109</v>
+      </c>
+      <c r="C14" t="s">
+        <v>147</v>
+      </c>
+      <c r="D14" s="3">
+        <v>41.878520999999999</v>
+      </c>
+      <c r="E14">
+        <v>-87.624853000000002</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>108</v>
-      </c>
-      <c r="D15" s="3"/>
+        <v>107</v>
+      </c>
+      <c r="C15" t="s">
+        <v>148</v>
+      </c>
+      <c r="D15" s="3">
+        <v>41.927098999999998</v>
+      </c>
+      <c r="E15">
+        <v>-87.630702999999997</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>121</v>
-      </c>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="C16" t="s">
+        <v>149</v>
+      </c>
+      <c r="D16" s="3">
+        <v>41.880815900000002</v>
+      </c>
+      <c r="E16">
+        <v>-87.7189628</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -1711,143 +1912,254 @@
         <v>102</v>
       </c>
       <c r="C17" t="s">
-        <v>124</v>
-      </c>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="D17" s="3">
+        <v>37.769421000000001</v>
+      </c>
+      <c r="E17">
+        <v>-122.486214</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>3</v>
       </c>
       <c r="B18" t="s">
         <v>104</v>
       </c>
-      <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>131</v>
+      </c>
+      <c r="D18" s="3">
+        <v>37.732840000000003</v>
+      </c>
+      <c r="E18">
+        <v>-122.50306500000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>3</v>
       </c>
       <c r="B19" t="s">
         <v>102</v>
       </c>
-      <c r="D19" s="3"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>127</v>
+      </c>
+      <c r="D19" s="3">
+        <v>37.772668000000003</v>
+      </c>
+      <c r="E19">
+        <v>-122.458758</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>3</v>
       </c>
       <c r="B20" t="s">
         <v>102</v>
       </c>
-      <c r="D20" s="3"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>129</v>
+      </c>
+      <c r="D20" s="3">
+        <v>37.801456000000002</v>
+      </c>
+      <c r="E20">
+        <v>-122.448053</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C21" t="s">
+        <v>121</v>
+      </c>
+      <c r="D21" s="3">
+        <v>37.808236999999998</v>
+      </c>
+      <c r="E21">
+        <v>-122.41574</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>109</v>
+      </c>
+      <c r="C22" t="s">
         <v>123</v>
       </c>
-      <c r="D21" s="3"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>3</v>
-      </c>
-      <c r="B22" t="s">
-        <v>110</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="D22" s="3">
+        <v>37.809305000000002</v>
+      </c>
+      <c r="E22">
+        <v>-122.416021</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>109</v>
+      </c>
+      <c r="C23" t="s">
+        <v>124</v>
+      </c>
+      <c r="D23" s="3">
+        <v>37.769865000000003</v>
+      </c>
+      <c r="E23">
+        <v>-122.466095</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" t="s">
+        <v>109</v>
+      </c>
+      <c r="C24" t="s">
+        <v>126</v>
+      </c>
+      <c r="D24" s="3">
+        <v>37.801394999999999</v>
+      </c>
+      <c r="E24">
+        <v>-122.45866100000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" t="s">
+        <v>115</v>
+      </c>
+      <c r="C25" t="s">
+        <v>133</v>
+      </c>
+      <c r="D25" s="3">
+        <v>37.819929000000002</v>
+      </c>
+      <c r="E25">
+        <v>-122.478255</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" t="s">
+        <v>132</v>
+      </c>
+      <c r="D26" s="3">
+        <v>37.764324000000002</v>
+      </c>
+      <c r="E26">
+        <v>-122.438408</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" t="s">
+        <v>115</v>
+      </c>
+      <c r="C27" t="s">
         <v>125</v>
       </c>
-      <c r="D22" s="3"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>3</v>
-      </c>
-      <c r="B23" t="s">
-        <v>110</v>
-      </c>
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>3</v>
-      </c>
-      <c r="B24" t="s">
-        <v>110</v>
-      </c>
-      <c r="D24" s="3"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25" t="s">
-        <v>102</v>
-      </c>
-      <c r="D25" s="3"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>3</v>
-      </c>
-      <c r="B26" t="s">
-        <v>110</v>
-      </c>
-      <c r="D26" s="3"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>3</v>
-      </c>
-      <c r="B27" t="s">
-        <v>116</v>
-      </c>
-      <c r="D27" s="3"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D27" s="3">
+        <v>37.826977999999997</v>
+      </c>
+      <c r="E27">
+        <v>-122.422956</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>102</v>
-      </c>
-      <c r="D28" s="3"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+      <c r="C28" t="s">
+        <v>130</v>
+      </c>
+      <c r="D28" s="3">
+        <v>37.802138999999997</v>
+      </c>
+      <c r="E28">
+        <v>-122.41874</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>110</v>
-      </c>
-      <c r="D29" s="3"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="C29" t="s">
+        <v>128</v>
+      </c>
+      <c r="D29" s="3">
+        <v>37.800856000000003</v>
+      </c>
+      <c r="E29">
+        <v>-122.398635</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>108</v>
-      </c>
-      <c r="D30" s="3"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="C30" t="s">
+        <v>134</v>
+      </c>
+      <c r="D30" s="3">
+        <v>37.762014000000001</v>
+      </c>
+      <c r="E30">
+        <v>-122.434924</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>121</v>
-      </c>
-      <c r="D31" s="3"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="C31" t="s">
+        <v>135</v>
+      </c>
+      <c r="D31" s="3">
+        <v>37.762014000000001</v>
+      </c>
+      <c r="E31">
+        <v>-122.434924</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>25</v>
       </c>
@@ -1857,9 +2169,14 @@
       <c r="C32" t="s">
         <v>103</v>
       </c>
-      <c r="D32" s="3"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D32" s="3">
+        <v>29.714874999999999</v>
+      </c>
+      <c r="E32">
+        <v>-95.389183000000003</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>25</v>
       </c>
@@ -1869,9 +2186,14 @@
       <c r="C33" t="s">
         <v>105</v>
       </c>
-      <c r="D33" s="3"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="3">
+        <v>29.71191</v>
+      </c>
+      <c r="E33">
+        <v>-95.392827999999994</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>25</v>
       </c>
@@ -1879,11 +2201,16 @@
         <v>102</v>
       </c>
       <c r="C34" t="s">
-        <v>106</v>
-      </c>
-      <c r="D34" s="3"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+      <c r="D34" s="3">
+        <v>29.737217999999999</v>
+      </c>
+      <c r="E34">
+        <v>-95.397064</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>25</v>
       </c>
@@ -1891,59 +2218,84 @@
         <v>102</v>
       </c>
       <c r="C35" t="s">
+        <v>106</v>
+      </c>
+      <c r="D35" s="3">
+        <v>29.754131999999998</v>
+      </c>
+      <c r="E35">
+        <v>-95.359909999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36" t="s">
         <v>107</v>
       </c>
-      <c r="D35" s="3"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>108</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" s="3">
+        <v>29.897554</v>
+      </c>
+      <c r="E36">
+        <v>-95.595483999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>25</v>
+      </c>
+      <c r="B37" t="s">
         <v>109</v>
       </c>
-      <c r="D36" s="3"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>25</v>
-      </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>110</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" s="3">
+        <v>29.550201000000001</v>
+      </c>
+      <c r="E37">
+        <v>-95.097012000000007</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>25</v>
+      </c>
+      <c r="B38" t="s">
+        <v>109</v>
+      </c>
+      <c r="C38" t="s">
         <v>111</v>
       </c>
-      <c r="D37" s="3"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>25</v>
-      </c>
-      <c r="B38" t="s">
-        <v>110</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="D38" s="3">
+        <v>29.772033</v>
+      </c>
+      <c r="E38">
+        <v>-95.396867</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39" t="s">
+        <v>109</v>
+      </c>
+      <c r="C39" t="s">
         <v>112</v>
       </c>
-      <c r="D38" s="3"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>25</v>
-      </c>
-      <c r="B39" t="s">
-        <v>110</v>
-      </c>
-      <c r="C39" t="s">
-        <v>113</v>
-      </c>
-      <c r="D39" s="3"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D39" s="3">
+        <v>29.717559000000001</v>
+      </c>
+      <c r="E39">
+        <v>-95.324261000000007</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>25</v>
       </c>
@@ -1951,35 +2303,50 @@
         <v>102</v>
       </c>
       <c r="C40" t="s">
+        <v>113</v>
+      </c>
+      <c r="D40" s="3">
+        <v>29.761621000000002</v>
+      </c>
+      <c r="E40">
+        <v>-95.393728999999993</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>25</v>
+      </c>
+      <c r="B41" t="s">
+        <v>109</v>
+      </c>
+      <c r="C41" t="s">
         <v>114</v>
       </c>
-      <c r="D40" s="3"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>25</v>
-      </c>
-      <c r="B41" t="s">
-        <v>110</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="D41" s="3">
+        <v>29.721819</v>
+      </c>
+      <c r="E41">
+        <v>-95.389702</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>25</v>
+      </c>
+      <c r="B42" t="s">
         <v>115</v>
       </c>
-      <c r="D41" s="3"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>25</v>
-      </c>
-      <c r="B42" t="s">
-        <v>116</v>
-      </c>
       <c r="C42" t="s">
-        <v>117</v>
-      </c>
-      <c r="D42" s="3"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+      <c r="D42" s="3">
+        <v>29.737151999999998</v>
+      </c>
+      <c r="E42">
+        <v>-95.461067999999997</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>25</v>
       </c>
@@ -1987,45 +2354,65 @@
         <v>102</v>
       </c>
       <c r="C43" t="s">
+        <v>116</v>
+      </c>
+      <c r="D43" s="3">
+        <v>29.761644</v>
+      </c>
+      <c r="E43">
+        <v>-95.377596999999994</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>25</v>
+      </c>
+      <c r="B44" t="s">
+        <v>109</v>
+      </c>
+      <c r="C44" t="s">
+        <v>117</v>
+      </c>
+      <c r="D44" s="3">
+        <v>29.73734</v>
+      </c>
+      <c r="E44">
+        <v>-95.398510000000002</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>25</v>
+      </c>
+      <c r="B45" t="s">
+        <v>107</v>
+      </c>
+      <c r="C45" t="s">
         <v>118</v>
       </c>
-      <c r="D43" s="3"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>25</v>
-      </c>
-      <c r="B44" t="s">
-        <v>110</v>
-      </c>
-      <c r="C44" t="s">
+      <c r="D45" s="3">
+        <v>29.736794</v>
+      </c>
+      <c r="E45">
+        <v>-95.397309000000007</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>25</v>
+      </c>
+      <c r="B46" t="s">
         <v>119</v>
       </c>
-      <c r="D44" s="3"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>25</v>
-      </c>
-      <c r="B45" t="s">
-        <v>108</v>
-      </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>120</v>
       </c>
-      <c r="D45" s="3"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>25</v>
-      </c>
-      <c r="B46" t="s">
-        <v>121</v>
-      </c>
-      <c r="C46" t="s">
-        <v>122</v>
-      </c>
-      <c r="D46" s="3"/>
+      <c r="D46" s="3">
+        <v>29.750767</v>
+      </c>
+      <c r="E46">
+        <v>-95.362036000000003</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added the remaining dummy data
</commit_message>
<xml_diff>
--- a/data/Dummy Data.xlsx
+++ b/data/Dummy Data.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\0001 MY COURSES\0000 Computer Science\COMP 346 - Internet Computing\346-term-project\Github\danglingpointers\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11145" windowHeight="11655" activeTab="1"/>
   </bookViews>
@@ -15,7 +10,10 @@
     <sheet name="Restaurants" sheetId="1" r:id="rId1"/>
     <sheet name="Attractions" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Attractions!$A$1:$E$46</definedName>
+  </definedNames>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -804,7 +802,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -814,8 +812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1048576"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1619,8 +1617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1654,16 +1652,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="C2" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="D2" s="3">
-        <v>41.882551999999997</v>
+        <v>41.882657000000002</v>
       </c>
       <c r="E2">
-        <v>-87.622551000000001</v>
+        <v>-87.623304000000005</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1671,16 +1669,16 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="C3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D3" s="3">
-        <v>41.92089</v>
+        <v>41.875793999999999</v>
       </c>
       <c r="E3">
-        <v>-87.632917000000006</v>
+        <v>-87.618948000000003</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1688,16 +1686,16 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="C4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D4" s="3">
-        <v>41.891641999999997</v>
+        <v>41.878875999999998</v>
       </c>
       <c r="E4">
-        <v>-87.605143999999996</v>
+        <v>-87.635914999999997</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1708,13 +1706,13 @@
         <v>115</v>
       </c>
       <c r="C5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D5" s="3">
-        <v>41.882657000000002</v>
+        <v>41.898510000000002</v>
       </c>
       <c r="E5">
-        <v>-87.623304000000005</v>
+        <v>-87.622765000000001</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1722,16 +1720,16 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C6" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="D6" s="3">
-        <v>42.031595000000003</v>
+        <v>41.790573000000002</v>
       </c>
       <c r="E6">
-        <v>-87.779088000000002</v>
+        <v>-87.583066000000002</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1742,13 +1740,13 @@
         <v>109</v>
       </c>
       <c r="C7" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D7" s="3">
-        <v>41.790573000000002</v>
+        <v>41.866261000000002</v>
       </c>
       <c r="E7">
-        <v>-87.583066000000002</v>
+        <v>-87.616979999999998</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1759,13 +1757,13 @@
         <v>109</v>
       </c>
       <c r="C8" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D8" s="3">
-        <v>41.866261000000002</v>
+        <v>41.883754000000003</v>
       </c>
       <c r="E8">
-        <v>-87.616979999999998</v>
+        <v>-87.624951999999993</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1776,13 +1774,13 @@
         <v>109</v>
       </c>
       <c r="C9" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D9" s="3">
-        <v>41.883754000000003</v>
+        <v>41.879584000000001</v>
       </c>
       <c r="E9">
-        <v>-87.624951999999993</v>
+        <v>-87.623712999999995</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1790,16 +1788,16 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C10" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="D10" s="3">
-        <v>41.875793999999999</v>
+        <v>41.878520999999999</v>
       </c>
       <c r="E10">
-        <v>-87.618948000000003</v>
+        <v>-87.624853000000002</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1807,16 +1805,16 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C11" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="D11" s="3">
-        <v>41.879584000000001</v>
+        <v>41.882551999999997</v>
       </c>
       <c r="E11">
-        <v>-87.623712999999995</v>
+        <v>-87.622551000000001</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1824,16 +1822,16 @@
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="C12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D12" s="3">
-        <v>41.878875999999998</v>
+        <v>41.891641999999997</v>
       </c>
       <c r="E12">
-        <v>-87.635914999999997</v>
+        <v>-87.605143999999996</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1841,16 +1839,16 @@
         <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C13" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="D13" s="3">
-        <v>41.898510000000002</v>
+        <v>41.880815900000002</v>
       </c>
       <c r="E13">
-        <v>-87.622765000000001</v>
+        <v>-87.7189628</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1858,16 +1856,16 @@
         <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C14" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="D14" s="3">
-        <v>41.878520999999999</v>
+        <v>42.031595000000003</v>
       </c>
       <c r="E14">
-        <v>-87.624853000000002</v>
+        <v>-87.779088000000002</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1892,529 +1890,534 @@
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="C16" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="D16" s="3">
-        <v>41.880815900000002</v>
+        <v>41.92089</v>
       </c>
       <c r="E16">
-        <v>-87.7189628</v>
+        <v>-87.632917000000006</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="C17" t="s">
-        <v>122</v>
+        <v>152</v>
       </c>
       <c r="D17" s="3">
-        <v>37.769421000000001</v>
+        <v>29.737151999999998</v>
       </c>
       <c r="E17">
-        <v>-122.486214</v>
+        <v>-95.461067999999997</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="C18" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="D18" s="3">
-        <v>37.732840000000003</v>
+        <v>29.550201000000001</v>
       </c>
       <c r="E18">
-        <v>-122.50306500000001</v>
+        <v>-95.097012000000007</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="C19" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="D19" s="3">
-        <v>37.772668000000003</v>
+        <v>29.772033</v>
       </c>
       <c r="E19">
-        <v>-122.458758</v>
+        <v>-95.396867</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="C20" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="D20" s="3">
-        <v>37.801456000000002</v>
+        <v>29.717559000000001</v>
       </c>
       <c r="E20">
-        <v>-122.448053</v>
+        <v>-95.324261000000007</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C21" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="D21" s="3">
-        <v>37.808236999999998</v>
+        <v>29.721819</v>
       </c>
       <c r="E21">
-        <v>-122.41574</v>
+        <v>-95.389702</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B22" t="s">
         <v>109</v>
       </c>
       <c r="C22" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D22" s="3">
-        <v>37.809305000000002</v>
+        <v>29.73734</v>
       </c>
       <c r="E22">
-        <v>-122.416021</v>
+        <v>-95.398510000000002</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C23" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="D23" s="3">
-        <v>37.769865000000003</v>
+        <v>29.714874999999999</v>
       </c>
       <c r="E23">
-        <v>-122.466095</v>
+        <v>-95.389183000000003</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C24" t="s">
-        <v>126</v>
+        <v>151</v>
       </c>
       <c r="D24" s="3">
-        <v>37.801394999999999</v>
+        <v>29.737217999999999</v>
       </c>
       <c r="E24">
-        <v>-122.45866100000001</v>
+        <v>-95.397064</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="C25" t="s">
-        <v>133</v>
+        <v>106</v>
       </c>
       <c r="D25" s="3">
-        <v>37.819929000000002</v>
+        <v>29.754131999999998</v>
       </c>
       <c r="E25">
-        <v>-122.478255</v>
+        <v>-95.359909999999999</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C26" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="D26" s="3">
-        <v>37.764324000000002</v>
+        <v>29.761621000000002</v>
       </c>
       <c r="E26">
-        <v>-122.438408</v>
+        <v>-95.393728999999993</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="C27" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="D27" s="3">
-        <v>37.826977999999997</v>
+        <v>29.761644</v>
       </c>
       <c r="E27">
-        <v>-122.422956</v>
+        <v>-95.377596999999994</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C28" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="D28" s="3">
-        <v>37.802138999999997</v>
+        <v>29.750767</v>
       </c>
       <c r="E28">
-        <v>-122.41874</v>
+        <v>-95.362036000000003</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B29" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C29" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="D29" s="3">
-        <v>37.800856000000003</v>
+        <v>29.897554</v>
       </c>
       <c r="E29">
-        <v>-122.398635</v>
+        <v>-95.595483999999999</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B30" t="s">
         <v>107</v>
       </c>
       <c r="C30" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="D30" s="3">
-        <v>37.762014000000001</v>
+        <v>29.736794</v>
       </c>
       <c r="E30">
-        <v>-122.434924</v>
+        <v>-95.397309000000007</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B31" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="C31" t="s">
-        <v>135</v>
+        <v>105</v>
       </c>
       <c r="D31" s="3">
-        <v>37.762014000000001</v>
+        <v>29.71191</v>
       </c>
       <c r="E31">
-        <v>-122.434924</v>
+        <v>-95.392827999999994</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B32" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="C32" t="s">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="D32" s="3">
-        <v>29.714874999999999</v>
+        <v>37.819929000000002</v>
       </c>
       <c r="E32">
-        <v>-95.389183000000003</v>
+        <v>-122.478255</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B33" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="C33" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="D33" s="3">
-        <v>29.71191</v>
+        <v>37.826977999999997</v>
       </c>
       <c r="E33">
-        <v>-95.392827999999994</v>
+        <v>-122.422956</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="C34" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="D34" s="3">
-        <v>29.737217999999999</v>
+        <v>37.802138999999997</v>
       </c>
       <c r="E34">
-        <v>-95.397064</v>
+        <v>-122.41874</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B35" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="C35" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="D35" s="3">
-        <v>29.754131999999998</v>
+        <v>37.809305000000002</v>
       </c>
       <c r="E35">
-        <v>-95.359909999999999</v>
+        <v>-122.416021</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B36" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C36" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="D36" s="3">
-        <v>29.897554</v>
+        <v>37.769865000000003</v>
       </c>
       <c r="E36">
-        <v>-95.595483999999999</v>
+        <v>-122.466095</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B37" t="s">
         <v>109</v>
       </c>
       <c r="C37" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="D37" s="3">
-        <v>29.550201000000001</v>
+        <v>37.801394999999999</v>
       </c>
       <c r="E37">
-        <v>-95.097012000000007</v>
+        <v>-122.45866100000001</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B38" t="s">
         <v>109</v>
       </c>
       <c r="C38" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="D38" s="3">
-        <v>29.772033</v>
+        <v>37.764324000000002</v>
       </c>
       <c r="E38">
-        <v>-95.396867</v>
+        <v>-122.438408</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B39" t="s">
         <v>109</v>
       </c>
       <c r="C39" t="s">
-        <v>112</v>
+        <v>128</v>
       </c>
       <c r="D39" s="3">
-        <v>29.717559000000001</v>
+        <v>37.800856000000003</v>
       </c>
       <c r="E39">
-        <v>-95.324261000000007</v>
+        <v>-122.398635</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B40" t="s">
         <v>102</v>
       </c>
       <c r="C40" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="D40" s="3">
-        <v>29.761621000000002</v>
+        <v>37.769421000000001</v>
       </c>
       <c r="E40">
-        <v>-95.393728999999993</v>
+        <v>-122.486214</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B41" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C41" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="D41" s="3">
-        <v>29.721819</v>
+        <v>37.772668000000003</v>
       </c>
       <c r="E41">
-        <v>-95.389702</v>
+        <v>-122.458758</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B42" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="C42" t="s">
-        <v>152</v>
+        <v>129</v>
       </c>
       <c r="D42" s="3">
-        <v>29.737151999999998</v>
+        <v>37.801456000000002</v>
       </c>
       <c r="E42">
-        <v>-95.461067999999997</v>
+        <v>-122.448053</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B43" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
       <c r="C43" t="s">
-        <v>116</v>
+        <v>135</v>
       </c>
       <c r="D43" s="3">
-        <v>29.761644</v>
+        <v>37.762014000000001</v>
       </c>
       <c r="E43">
-        <v>-95.377596999999994</v>
+        <v>-122.434924</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B44" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C44" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="D44" s="3">
-        <v>29.73734</v>
+        <v>37.808236999999998</v>
       </c>
       <c r="E44">
-        <v>-95.398510000000002</v>
+        <v>-122.41574</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B45" t="s">
         <v>107</v>
       </c>
       <c r="C45" t="s">
-        <v>118</v>
+        <v>134</v>
       </c>
       <c r="D45" s="3">
-        <v>29.736794</v>
+        <v>37.762014000000001</v>
       </c>
       <c r="E45">
-        <v>-95.397309000000007</v>
+        <v>-122.434924</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B46" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="C46" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="D46" s="3">
-        <v>29.750767</v>
+        <v>37.732840000000003</v>
       </c>
       <c r="E46">
-        <v>-95.362036000000003</v>
+        <v>-122.50306500000001</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E46">
+    <sortState ref="A2:E46">
+      <sortCondition ref="A1:A46"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>